<commit_message>
add create diary page remove keyword portal
</commit_message>
<xml_diff>
--- a/neo_server/rsc/neoserver_page_info.xlsx
+++ b/neo_server/rsc/neoserver_page_info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\PYSERVER\src\neo_server\rsc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\neo_server\neo_server\rsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380DE6FF-33AC-4317-B6C9-E7A5D19E2564}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="38280" yWindow="5175" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
   <si>
     <t>webtoon</t>
   </si>
@@ -74,15 +75,9 @@
     <t>keyword_order</t>
   </si>
   <si>
-    <t>포탈 검색순위</t>
-  </si>
-  <si>
     <t>kwo</t>
   </si>
   <si>
-    <t>각 포털의 검색어 순위를 보는 사이트 입니다.</t>
-  </si>
-  <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,10 +133,6 @@
   </si>
   <si>
     <t>PasswdWebApp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KeywordOrderWebApp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -313,10 +304,6 @@
   </si>
   <si>
     <t>/today_contents.neo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/keyword_order.neo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -472,11 +459,33 @@
 )</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>원석의 일기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/create_diary.neo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_diary</t>
+  </si>
+  <si>
+    <t>CreateDiaryWebApp</t>
+  </si>
+  <si>
+    <t>개인 일기 제목 자동 생성 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_diary.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -836,14 +845,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -864,57 +873,57 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
       <c r="M1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="165" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -926,89 +935,92 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="231" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="231" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" t="s">
-        <v>76</v>
-      </c>
       <c r="H4" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.3">
@@ -1016,19 +1028,19 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -1037,19 +1049,19 @@
         <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="152.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1057,13 +1069,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
@@ -1075,33 +1087,33 @@
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="198" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -1113,19 +1125,19 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1136,7 +1148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1150,19 +1162,19 @@
   <sheetData>
     <row r="1" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>57</v>
-      </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -1174,16 +1186,16 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1204,62 +1216,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1281,19 +1293,19 @@
   <sheetData>
     <row r="1" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -1305,16 +1317,16 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -1322,16 +1334,16 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -1343,19 +1355,19 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>